<commit_message>
modify RandomUtil.py and MockExamUtil.py
</commit_message>
<xml_diff>
--- a/resources/mockExam/题库模版.xlsx
+++ b/resources/mockExam/题库模版.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowHeight="14300"/>
+    <workbookView windowHeight="14300" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="考试信息" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67">
   <si>
     <t>科目名称</t>
   </si>
@@ -52,6 +52,9 @@
     <t>答案</t>
   </si>
   <si>
+    <t>备注</t>
+  </si>
+  <si>
     <t>解析</t>
   </si>
   <si>
@@ -79,6 +82,30 @@
     <t>选项H</t>
   </si>
   <si>
+    <t>女子运动取消</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>是</t>
+  </si>
+  <si>
+    <t>否</t>
+  </si>
+  <si>
+    <t>中国夺冠</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>对的</t>
+  </si>
+  <si>
+    <t>错的</t>
+  </si>
+  <si>
     <t>完整的计算机系统由（）组成。</t>
   </si>
   <si>
@@ -160,9 +187,6 @@
     <t>下列设备中，属于输出设备的是（）。</t>
   </si>
   <si>
-    <t>A</t>
-  </si>
-  <si>
     <t>下列设备中，属于输出设备的是显示器。</t>
   </si>
   <si>
@@ -176,6 +200,24 @@
   </si>
   <si>
     <t>手字板</t>
+  </si>
+  <si>
+    <t>下列设备哪些是输入设备</t>
+  </si>
+  <si>
+    <t>ABD</t>
+  </si>
+  <si>
+    <t>键盘</t>
+  </si>
+  <si>
+    <t>鼠标</t>
+  </si>
+  <si>
+    <t>显示器</t>
+  </si>
+  <si>
+    <t>写字板</t>
   </si>
 </sst>
 </file>
@@ -1139,14 +1181,13 @@
   <sheetPr/>
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView zoomScale="150" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="17.6" outlineLevelRow="1" outlineLevelCol="7"/>
   <cols>
-    <col min="1" max="1" width="12.5714285714286" customWidth="1"/>
-    <col min="3" max="8" width="12.5714285714286" customWidth="1"/>
+    <col min="1" max="8" width="16.6428571428571" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -1210,15 +1251,21 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:L3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="A1" sqref="A$1:A$1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="17.6"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="17.6" outlineLevelRow="2"/>
+  <cols>
+    <col min="1" max="1" width="48.6428571428571" customWidth="1"/>
+    <col min="2" max="2" width="8.64285714285714" customWidth="1"/>
+    <col min="3" max="3" width="16.6428571428571" customWidth="1"/>
+    <col min="4" max="12" width="16.6428571428571" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -1252,8 +1299,44 @@
       <c r="K1" t="s">
         <v>19</v>
       </c>
+      <c r="L1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" t="s">
+        <v>22</v>
+      </c>
+      <c r="E2" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+      <c r="E3" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" t="s">
+        <v>28</v>
+      </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C4 C5:C6">
+      <formula1>"A,B,C,D,E,F,G,H"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
 </worksheet>
@@ -1262,23 +1345,20 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:L6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="$A1:$XFD1"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="17.6" outlineLevelRow="5"/>
   <cols>
-    <col min="1" max="1" width="48.8035714285714" customWidth="1"/>
-    <col min="3" max="3" width="10.1428571428571" customWidth="1"/>
-    <col min="4" max="4" width="19.0714285714286" customWidth="1"/>
-    <col min="5" max="5" width="29.4285714285714" customWidth="1"/>
-    <col min="6" max="6" width="33.4285714285714" customWidth="1"/>
-    <col min="7" max="7" width="27.0714285714286" customWidth="1"/>
+    <col min="1" max="1" width="48.6428571428571" customWidth="1"/>
+    <col min="2" max="2" width="8.64285714285714" customWidth="1"/>
+    <col min="3" max="12" width="16.6428571428571" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -1312,125 +1392,128 @@
       <c r="K1" t="s">
         <v>19</v>
       </c>
+      <c r="L1" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:8">
       <c r="A2" s="1" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="B2" t="s">
-        <v>21</v>
-      </c>
-      <c r="C2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>23</v>
+        <v>30</v>
+      </c>
+      <c r="D2" t="s">
+        <v>31</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>25</v>
+        <v>33</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8">
+      <c r="A3" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8">
+      <c r="A4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D4" t="s">
+        <v>44</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D5" t="s">
+        <v>50</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F5" t="s">
+        <v>52</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B6" t="s">
         <v>26</v>
       </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="B3" t="s">
-        <v>28</v>
-      </c>
-      <c r="C3" t="s">
-        <v>29</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>30</v>
-      </c>
-      <c r="E3" s="2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C4" t="s">
-        <v>35</v>
-      </c>
-      <c r="D4" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="A5" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="B5" t="s">
-        <v>21</v>
-      </c>
-      <c r="C5" t="s">
-        <v>41</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="E5" t="s">
-        <v>43</v>
-      </c>
-      <c r="F5" s="2" t="s">
-        <v>44</v>
-      </c>
-      <c r="G5" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="A6" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="B6" t="s">
-        <v>47</v>
-      </c>
-      <c r="C6" t="s">
-        <v>48</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="E6" t="s">
-        <v>50</v>
+      <c r="D6" t="s">
+        <v>56</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>57</v>
       </c>
       <c r="F6" t="s">
-        <v>51</v>
+        <v>58</v>
       </c>
       <c r="G6" t="s">
-        <v>52</v>
+        <v>59</v>
+      </c>
+      <c r="H6" t="s">
+        <v>60</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B4 B5:B6">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B2:B4 B5:B6 C2:C4 C5:C6">
       <formula1>"A,B,C,D,E,F,G,H"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1442,15 +1525,21 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr/>
-  <dimension ref="A1:K1"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="17.6"/>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="17.6" outlineLevelRow="1"/>
+  <cols>
+    <col min="1" max="1" width="48.6428571428571" customWidth="1"/>
+    <col min="2" max="2" width="8.64285714285714" customWidth="1"/>
+    <col min="3" max="3" width="16.6428571428571" customWidth="1"/>
+    <col min="4" max="12" width="16.6428571428571" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:11">
+    <row r="1" spans="1:12">
       <c r="A1" t="s">
         <v>9</v>
       </c>
@@ -1484,8 +1573,36 @@
       <c r="K1" t="s">
         <v>19</v>
       </c>
+      <c r="L1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8">
+      <c r="A2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F2" t="s">
+        <v>64</v>
+      </c>
+      <c r="G2" t="s">
+        <v>65</v>
+      </c>
+      <c r="H2" t="s">
+        <v>66</v>
+      </c>
     </row>
   </sheetData>
+  <dataValidations count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C2:C4 C5:C6">
+      <formula1>"A,B,C,D,E,F,G,H"</formula1>
+    </dataValidation>
+  </dataValidations>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.511805555555556" footer="0.511805555555556"/>
   <headerFooter/>
 </worksheet>

</xml_diff>